<commit_message>
Fix: tomato raw data
</commit_message>
<xml_diff>
--- a/MicroFarm/Data/Tomato/2022_tomato_Growing-Info_Daily.xlsx
+++ b/MicroFarm/Data/Tomato/2022_tomato_Growing-Info_Daily.xlsx
@@ -239,17 +239,17 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>2022-04-11</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t>150.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
@@ -264,17 +264,17 @@
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>236.0</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>174.0</t>
         </is>
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -301,47 +301,47 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>2022-04-18</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>85.0</t>
+          <t>240.0</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>105.0</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>290.0</t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>237.0</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J4" s="4" t="inlineStr">
@@ -356,453 +356,453 @@
       </c>
       <c r="L4" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>2.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>2022-04-25</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>323.0</t>
+          <t>316.0</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>127.0</t>
+          <t>134.0</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>268.0</t>
+          <t>385.0</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>220.0</t>
+          <t>308.0</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I5" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="J5" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="K5" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="L5" s="4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>3.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>2022-05-02</t>
+          <t>2022-04-20</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>213.0</t>
+          <t>262.0</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>393.0</t>
+          <t>161.0</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>285.0</t>
+          <t>536.0</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>260.0</t>
+          <t>397.0</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="J6" s="4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="K6" s="4" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="L6" s="4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>2022-05-09</t>
+          <t>2022-04-27</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>313.0</t>
+          <t>289.0</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>99.0</t>
+          <t>138.0</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>503.0</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>345.0</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>12.0</t>
+        </is>
+      </c>
+      <c r="I7" s="4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="K7" s="4" t="inlineStr">
+        <is>
           <t>11.0</t>
         </is>
       </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>343.0</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>333.0</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>9.0</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
       <c r="L7" s="4" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>2022-05-18</t>
+          <t>2022-05-04</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>316.0</t>
+          <t>243.0</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>149.0</t>
+          <t>78.0</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>430.0</t>
+          <t>455.0</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>335.0</t>
+          <t>295.0</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
+          <t>11.0</t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="J8" s="4" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="K8" s="4" t="inlineStr">
+        <is>
           <t>13.0</t>
         </is>
       </c>
-      <c r="I8" s="4" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="J8" s="4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="K8" s="4" t="inlineStr">
-        <is>
-          <t>11.0</t>
-        </is>
-      </c>
       <c r="L8" s="4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>2022-05-23</t>
+          <t>2022-05-11</t>
         </is>
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>259.0</t>
+          <t>268.0</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>290.0</t>
+          <t>205.0</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>466.0</t>
+          <t>493.0</t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>356.0</t>
+          <t>423.0</t>
         </is>
       </c>
       <c r="H9" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="I9" s="4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="J9" s="4" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="K9" s="4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>2022-05-30</t>
+          <t>2022-05-18</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>250.0</t>
+          <t>204.0</t>
         </is>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>300.0</t>
+          <t>131.0</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>416.0</t>
+          <t>498.0</t>
         </is>
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>400.0</t>
+          <t>403.0</t>
         </is>
       </c>
       <c r="H10" s="4" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="I10" s="4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="J10" s="4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="K10" s="4" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>14.0</t>
         </is>
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>7.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>2022-06-07</t>
+          <t>2022-05-25</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>280.0</t>
+          <t>244.0</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>230.0</t>
+          <t>99.0</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>408.0</t>
+          <t>476.0</t>
         </is>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>363.0</t>
+          <t>413.0</t>
         </is>
       </c>
       <c r="H11" s="4" t="inlineStr">
         <is>
-          <t>18.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I11" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="J11" s="4" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="K11" s="4" t="inlineStr">
         <is>
-          <t>21.0</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>8.0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>2022-06-14</t>
+          <t>2022-06-01</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>176.0</t>
+          <t>196.0</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -822,280 +822,280 @@
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>383.0</t>
+          <t>476.0</t>
         </is>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>248.0</t>
+          <t>413.0</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="J12" s="4" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="K12" s="4" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="L12" s="4" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>9.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>2022-06-21</t>
+          <t>2022-06-08</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>303.0</t>
+          <t>193.0</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>173.0</t>
+          <t>249.0</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>490.0</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>445.0</t>
+        </is>
+      </c>
+      <c r="H13" s="4" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="I13" s="4" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="J13" s="4" t="inlineStr">
+        <is>
           <t>8.0</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>395.0</t>
-        </is>
-      </c>
-      <c r="G13" s="4" t="inlineStr">
-        <is>
-          <t>300.0</t>
-        </is>
-      </c>
-      <c r="H13" s="4" t="inlineStr">
-        <is>
-          <t>22.0</t>
-        </is>
-      </c>
-      <c r="I13" s="4" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="J13" s="4" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
       <c r="K13" s="4" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="L13" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>9.0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>2022-06-29</t>
+          <t>2022-06-15</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>274.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>129.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>420.0</t>
+          <t>581.0</t>
         </is>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>313.0</t>
+          <t>513.0</t>
         </is>
       </c>
       <c r="H14" s="4" t="inlineStr">
         <is>
-          <t>25.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I14" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="J14" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="K14" s="4" t="inlineStr">
         <is>
-          <t>24.0</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="L14" s="4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>2022-07-06</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>313.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>290.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>390.0</t>
+          <t>598.0</t>
         </is>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>305.0</t>
+          <t>533.0</t>
         </is>
       </c>
       <c r="H15" s="4" t="inlineStr">
         <is>
-          <t>26.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="L15" s="4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>2022-07-14</t>
+          <t>2022-06-29</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>258.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>278.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>425.0</t>
+          <t>563.0</t>
         </is>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>345.0</t>
+          <t>486.0</t>
         </is>
       </c>
       <c r="H16" s="4" t="inlineStr">
         <is>
-          <t>26.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I16" s="4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J16" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="K16" s="4" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="L16" s="4" t="inlineStr">
@@ -1107,193 +1107,193 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>2022-07-21</t>
+          <t>2022-07-06</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>244.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>245.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>355.0</t>
+          <t>566.0</t>
         </is>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>265.0</t>
+          <t>492.0</t>
         </is>
       </c>
       <c r="H17" s="4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I17" s="4" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J17" s="4" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="K17" s="4" t="inlineStr">
+        <is>
           <t>11.0</t>
         </is>
       </c>
-      <c r="J17" s="4" t="inlineStr">
-        <is>
-          <t>9.0</t>
-        </is>
-      </c>
-      <c r="K17" s="4" t="inlineStr">
-        <is>
-          <t>12.0</t>
-        </is>
-      </c>
       <c r="L17" s="4" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>2022-07-28</t>
+          <t>2022-07-13</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>228.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>158.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>370.0</t>
+          <t>570.0</t>
         </is>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>275.0</t>
+          <t>521.0</t>
         </is>
       </c>
       <c r="H18" s="4" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="L18" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>2022-08-04</t>
+          <t>2022-07-20</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>205.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>138.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="F19" s="4" t="inlineStr">
         <is>
-          <t>323.0</t>
+          <t>575.0</t>
         </is>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>220.0</t>
+          <t>525.0</t>
         </is>
       </c>
       <c r="H19" s="4" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="I19" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J19" s="4" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="K19" s="4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="L19" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>2022-08-12</t>
+          <t>2022-07-27</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
@@ -1303,176 +1303,52 @@
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>178.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>320.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>330.0</t>
+          <t>581.0</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>240.0</t>
+          <t>538.0</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="L20" s="4" t="inlineStr">
         <is>
-          <t>14.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>2022-08-19</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>179.0</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="inlineStr">
-        <is>
-          <t>300.0</t>
-        </is>
-      </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>338.0</t>
-        </is>
-      </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>253.0</t>
-        </is>
-      </c>
-      <c r="H21" s="4" t="inlineStr">
-        <is>
-          <t>13.0</t>
-        </is>
-      </c>
-      <c r="I21" s="4" t="inlineStr">
-        <is>
-          <t>13.0</t>
-        </is>
-      </c>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>12.0</t>
-        </is>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
-      <c r="L21" s="4" t="inlineStr">
-        <is>
-          <t>14.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>2022-08-26</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>177.0</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="inlineStr">
-        <is>
-          <t>280.0</t>
-        </is>
-      </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
-        <is>
-          <t>355.0</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>265.0</t>
-        </is>
-      </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>14.0</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>14.0</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>13.0</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>15.0</t>
+          <t>10.0</t>
         </is>
       </c>
     </row>

</xml_diff>